<commit_message>
ci: :bookmark: up to v1.0.2
</commit_message>
<xml_diff>
--- a/user2.xlsx
+++ b/user2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>name</t>
   </si>
@@ -36,6 +36,12 @@
   </si>
   <si>
     <t>shanghai</t>
+  </si>
+  <si>
+    <t>rose</t>
+  </si>
+  <si>
+    <t>beijing</t>
   </si>
 </sst>
 </file>
@@ -80,7 +86,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -120,6 +126,40 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="n">
+        <v>12000.0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="n">
+        <v>29.0</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="n">
+        <v>11111.1</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>